<commit_message>
Updated application with new changes
</commit_message>
<xml_diff>
--- a/locations/A01.xlsx
+++ b/locations/A01.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://comlineukcom-my.sharepoint.com/personal/jaydip_d_comline_uk_com/Documents/CAPLOCATION/bulk_report_webapp/locations/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://comlineukcom-my.sharepoint.com/personal/jaydip_d_comline_uk_com/Documents/CAPLOCATION/Deployment/bulk_report_webapp/locations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{356FF99A-966F-40C2-A35E-C20F8A6CCBCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0FF1E1F-29E4-480C-BA4B-A2ED7D8DE2C7}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{356FF99A-966F-40C2-A35E-C20F8A6CCBCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{285B657B-27D8-49A1-B0B7-1CA5B3358EB7}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1253,7 +1253,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1315,11 +1315,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1371,7 +1391,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1387,10 +1412,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1714,7 +1735,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C14" sqref="C14"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1813,8 +1834,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A2" s="16" t="s">
+    <row r="2" spans="1:30" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
@@ -1902,7 +1923,7 @@
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A3" s="17"/>
+      <c r="A3" s="20"/>
       <c r="B3" s="9"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -1934,7 +1955,7 @@
       <c r="AD3" s="7"/>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A4" s="17"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="9" t="s">
         <v>29</v>
       </c>
@@ -2020,7 +2041,7 @@
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A5" s="17"/>
+      <c r="A5" s="20"/>
       <c r="B5" s="9"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -2052,7 +2073,7 @@
       <c r="AD5" s="7"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A6" s="17"/>
+      <c r="A6" s="20"/>
       <c r="B6" s="9" t="s">
         <v>56</v>
       </c>
@@ -2138,7 +2159,7 @@
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A7" s="17"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="9"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -2170,7 +2191,7 @@
       <c r="AD7" s="7"/>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A8" s="17"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="9" t="s">
         <v>83</v>
       </c>
@@ -2256,7 +2277,7 @@
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A9" s="17"/>
+      <c r="A9" s="20"/>
       <c r="B9" s="9"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -2288,7 +2309,7 @@
       <c r="AD9" s="7"/>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A10" s="17"/>
+      <c r="A10" s="20"/>
       <c r="B10" s="9" t="s">
         <v>110</v>
       </c>
@@ -2374,7 +2395,7 @@
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A11" s="17"/>
+      <c r="A11" s="20"/>
       <c r="B11" s="9"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -2406,7 +2427,7 @@
       <c r="AD11" s="7"/>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A12" s="17"/>
+      <c r="A12" s="20"/>
       <c r="B12" s="9" t="s">
         <v>137</v>
       </c>
@@ -2492,7 +2513,7 @@
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A13" s="17"/>
+      <c r="A13" s="20"/>
       <c r="B13" s="9"/>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
@@ -2524,7 +2545,7 @@
       <c r="AD13" s="13"/>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A14" s="19"/>
+      <c r="A14" s="20"/>
       <c r="B14" s="9" t="s">
         <v>164</v>
       </c>
@@ -2610,7 +2631,7 @@
       </c>
     </row>
     <row r="15" spans="1:30" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="19"/>
+      <c r="A15" s="20"/>
       <c r="B15" s="9"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -3709,8 +3730,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A2:A13"/>
     <mergeCell ref="A18:A31"/>
+    <mergeCell ref="A2:A15"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape"/>

</xml_diff>